<commit_message>
Finally got rid of health bar bug!
Health bar bug removed and remodeled. Also added general housekeeping
health things (can't exceed max, dead if 0 or under ect)
</commit_message>
<xml_diff>
--- a/Assets/Spredsheets/wanted.xlsx
+++ b/Assets/Spredsheets/wanted.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Attack</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Hired Muscle</t>
   </si>
   <si>
-    <t>Career Criminal</t>
-  </si>
-  <si>
     <t>Professional</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
   </si>
   <si>
     <t>Violent Crime</t>
-  </si>
-  <si>
-    <t>Criminal-damage-arson</t>
   </si>
   <si>
     <t>Drugs</t>
@@ -628,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H23"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,10 +638,10 @@
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
@@ -670,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -694,7 +688,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -718,7 +712,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1">
         <v>-1</v>
@@ -741,7 +735,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -767,115 +761,92 @@
         <v>27</v>
       </c>
       <c r="D7" s="1">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="H7" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="8">
         <v>-3</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="G8" s="8">
         <v>130</v>
       </c>
-      <c r="H8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>2</v>
-      </c>
-      <c r="F9" s="8">
-        <v>-3</v>
-      </c>
-      <c r="G9" s="8">
-        <v>130</v>
-      </c>
-      <c r="H9" s="9">
-        <v>0</v>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>